<commit_message>
Compared the calculated data to an accurate database - Google Maps Interactive Maps for Solar Eclipses [XJubier]...
</commit_message>
<xml_diff>
--- a/DATAFRAME (SOLAR_ECLIPSE_SAFARI) [LAT_LONG].xlsx
+++ b/DATAFRAME (SOLAR_ECLIPSE_SAFARI) [LAT_LONG].xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="8" documentId="8_{C121EA72-5276-4138-BDAB-CF3BA78EC397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69A8219F-D56F-4568-AADF-ED17AECA438C}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{602ED0A7-C94D-4A27-94C9-3E2CC28CA24C}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{602ED0A7-C94D-4A27-94C9-3E2CC28CA24C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1207,6 +1207,10 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1509,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D455B3-9B0E-4216-BCA6-CFE19CBF2F9A}">
   <dimension ref="A1:H684"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H320" workbookViewId="0">
-      <selection activeCell="L341" sqref="A341:XFD341"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>